<commit_message>
inicio da continuacao backend 06-07
</commit_message>
<xml_diff>
--- a/0_Diversos_ArquivosDeApoio/Relatorios_-_Daily_Trello.xlsx
+++ b/0_Diversos_ArquivosDeApoio/Relatorios_-_Daily_Trello.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t xml:space="preserve">ATIVIDADES</t>
   </si>
@@ -41,6 +41,17 @@
     <t xml:space="preserve">finalizar front end Editar Perfil</t>
   </si>
   <si>
+    <t xml:space="preserve">inicio backend Usuario
+Junção dos conteudos nas 
+Branches github</t>
+  </si>
+  <si>
+    <t xml:space="preserve">backend Usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">finalização Usuario</t>
+  </si>
+  <si>
     <t xml:space="preserve">Felipe</t>
   </si>
   <si>
@@ -57,10 +68,16 @@
     <t xml:space="preserve">Finalizar FrontEnd Feed</t>
   </si>
   <si>
+    <t xml:space="preserve">backend Post</t>
+  </si>
+  <si>
     <t xml:space="preserve">Andrey</t>
   </si>
   <si>
     <t xml:space="preserve">Back End Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BackEnd Login</t>
   </si>
   <si>
     <t xml:space="preserve">Geovanna</t>
@@ -85,10 +102,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -162,7 +178,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -172,10 +188,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -200,19 +212,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:E8"/>
+  <dimension ref="A3:H8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="25.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.86"/>
   </cols>
   <sheetData>
     <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -228,72 +242,105 @@
       <c r="D3" s="2" t="n">
         <v>44377</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="2" t="n">
         <v>44378</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>44379</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>44382</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>44383</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="F4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>